<commit_message>
PWA_REV2, Added a tab to seperate purchases by distributor type.
</commit_message>
<xml_diff>
--- a/PWA_REV2/RAW_PWA_REV2KiCad6_250910_1400.xlsx
+++ b/PWA_REV2/RAW_PWA_REV2KiCad6_250910_1400.xlsx
@@ -5,23 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac7503edfc2610fe/Desktop/PPF/PbF/4pi/Esp32BasedProjects/krake/PWA_REV2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop Pro\OneDrive\Desktop\PPF\PbF\4pi\Esp32BasedProjects\krake\PWA_REV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{DE9CB3E1-2886-4473-852D-FA2BCC0C6545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9901004D-AFD1-4A6A-933D-64386E0969EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEACD947-720E-48AC-9515-4B8FE8746F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4935" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4935" windowWidth="21840" windowHeight="13020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PWA_REV2KiCad6_250910_1303" sheetId="1" r:id="rId1"/>
-    <sheet name="PCBWAY_BOM" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Nagham_ElectrosLab" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="PCBWAY_BOM" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3765" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="664">
   <si>
     <t>Source:</t>
   </si>
@@ -2079,6 +2082,12 @@
   </si>
   <si>
     <t>2Mbps 3.3V Transceiver USB 2.0 SOP-16 USB Converters ROHS</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distributor Contact info: </t>
   </si>
 </sst>
 </file>
@@ -2244,7 +2253,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2436,8 +2445,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -2587,6 +2608,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2635,7 +2704,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2650,6 +2719,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2696,7 +2776,82 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2755,6 +2910,17 @@
     <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Sim.Enable"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Status"/>
     <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5B847B7-EE49-452A-99A5-68F886376DBD}" name="Table2" displayName="Table2" ref="A1:B7" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:B7" xr:uid="{D5B847B7-EE49-452A-99A5-68F886376DBD}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{AEF86317-4946-476A-9BE0-12817D74164E}" name="QTY" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{F6414858-8C7C-4CEC-B39E-C6F2F86C0BEB}" name="Item" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3059,8 +3225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H230" workbookViewId="0">
-      <selection activeCell="I288" sqref="I288"/>
+    <sheetView topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="A232" sqref="A232:AA308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15418,6 +15584,1116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF64B81-30C2-4AFE-9C6A-A04BAD9C3148}">
+  <dimension ref="A1:AA17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22:J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="7" width="8.7265625" customWidth="1"/>
+    <col min="14" max="14" width="19.26953125" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="29.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="12">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="14"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="12">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9">
+        <v>3.33</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="14"/>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="12">
+        <v>41</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9">
+        <v>7.11</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="14"/>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="12">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.36</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA5" s="14"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="12">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.65</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="U6" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA6" s="14"/>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="12">
+        <v>25</v>
+      </c>
+      <c r="B7" s="9">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9">
+        <v>4694</v>
+      </c>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="14"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="12">
+        <v>32</v>
+      </c>
+      <c r="B8" s="9">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9">
+        <v>1.5E-3</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="14"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="12">
+        <v>73</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9">
+        <v>4.99</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>403534100457</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="14"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" s="12">
+        <v>23</v>
+      </c>
+      <c r="B10" s="9">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="14"/>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" s="12">
+        <v>24</v>
+      </c>
+      <c r="B11" s="9">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9">
+        <v>0.1145</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="14"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" s="12">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9">
+        <v>0</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="14"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" s="12">
+        <v>22</v>
+      </c>
+      <c r="B13" s="9">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="14"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" s="12">
+        <v>44</v>
+      </c>
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="14"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" s="12">
+        <v>26</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="14"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" s="12">
+        <v>27</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="14"/>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" s="17">
+        <v>43</v>
+      </c>
+      <c r="B17" s="18">
+        <v>1</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19FF898-6F4B-4867-B17E-45B5E2D43CBC}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="120.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="9">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>599</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8E61AB-16C5-45E5-BF34-9C7D74F0C910}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:I63"/>
   <sheetViews>

</xml_diff>

<commit_message>
RAW_PWA_REV2KiCad6_250910_1400, adding BOM list.
</commit_message>
<xml_diff>
--- a/PWA_REV2/RAW_PWA_REV2KiCad6_250910_1400.xlsx
+++ b/PWA_REV2/RAW_PWA_REV2KiCad6_250910_1400.xlsx
@@ -5,23 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac7503edfc2610fe/Desktop/PPF/PbF/4pi/Esp32BasedProjects/krake/PWA_REV2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laptop Pro\OneDrive\Desktop\PPF\PbF\4pi\Esp32BasedProjects\krake\PWA_REV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{DE9CB3E1-2886-4473-852D-FA2BCC0C6545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9901004D-AFD1-4A6A-933D-64386E0969EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEACD947-720E-48AC-9515-4B8FE8746F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4935" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4935" windowWidth="21840" windowHeight="13020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PWA_REV2KiCad6_250910_1303" sheetId="1" r:id="rId1"/>
-    <sheet name="PCBWAY_BOM" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Nagham_ElectrosLab" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="PCBWAY_BOM" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3765" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="664">
   <si>
     <t>Source:</t>
   </si>
@@ -2079,6 +2082,12 @@
   </si>
   <si>
     <t>2Mbps 3.3V Transceiver USB 2.0 SOP-16 USB Converters ROHS</t>
+  </si>
+  <si>
+    <t>QTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distributor Contact info: </t>
   </si>
 </sst>
 </file>
@@ -2244,7 +2253,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2436,8 +2445,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -2587,6 +2608,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2635,7 +2704,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2650,6 +2719,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2696,7 +2776,82 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2755,6 +2910,17 @@
     <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Sim.Enable"/>
     <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Status"/>
     <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5B847B7-EE49-452A-99A5-68F886376DBD}" name="Table2" displayName="Table2" ref="A1:B7" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A1:B7" xr:uid="{D5B847B7-EE49-452A-99A5-68F886376DBD}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{AEF86317-4946-476A-9BE0-12817D74164E}" name="QTY" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{F6414858-8C7C-4CEC-B39E-C6F2F86C0BEB}" name="Item" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3059,8 +3225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA308"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H230" workbookViewId="0">
-      <selection activeCell="I288" sqref="I288"/>
+    <sheetView topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="A232" sqref="A232:AA308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15418,6 +15584,1116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF64B81-30C2-4AFE-9C6A-A04BAD9C3148}">
+  <dimension ref="A1:AA17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22:J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="7" width="8.7265625" customWidth="1"/>
+    <col min="14" max="14" width="19.26953125" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="17" width="29.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="12">
+        <v>2</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="Z2" s="9"/>
+      <c r="AA2" s="14"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="12">
+        <v>19</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9">
+        <v>3.33</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="14"/>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="12">
+        <v>41</v>
+      </c>
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9">
+        <v>7.11</v>
+      </c>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="14"/>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="12">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.36</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="U5" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA5" s="14"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="12">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9">
+        <v>5</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.65</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="O6" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q6" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="U6" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA6" s="14"/>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="12">
+        <v>25</v>
+      </c>
+      <c r="B7" s="9">
+        <v>4</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9">
+        <v>4694</v>
+      </c>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="14"/>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" s="12">
+        <v>32</v>
+      </c>
+      <c r="B8" s="9">
+        <v>4</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9">
+        <v>1.5E-3</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="14"/>
+    </row>
+    <row r="9" spans="1:27">
+      <c r="A9" s="12">
+        <v>73</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9">
+        <v>4.99</v>
+      </c>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>403534100457</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="14"/>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="A10" s="12">
+        <v>23</v>
+      </c>
+      <c r="B10" s="9">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9">
+        <v>1.8200000000000001E-2</v>
+      </c>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="14"/>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11" s="12">
+        <v>24</v>
+      </c>
+      <c r="B11" s="9">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>638</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9">
+        <v>0.1145</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q11" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="14"/>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12" s="12">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9">
+        <v>0</v>
+      </c>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="14"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" s="12">
+        <v>22</v>
+      </c>
+      <c r="B13" s="9">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>636</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="14"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" s="12">
+        <v>44</v>
+      </c>
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>499</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>500</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="14"/>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" s="12">
+        <v>26</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="14"/>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" s="12">
+        <v>27</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9">
+        <v>1000000</v>
+      </c>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="14"/>
+    </row>
+    <row r="17" spans="1:27">
+      <c r="A17" s="17">
+        <v>43</v>
+      </c>
+      <c r="B17" s="18">
+        <v>1</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19FF898-6F4B-4867-B17E-45B5E2D43CBC}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="17.7265625" customWidth="1"/>
+    <col min="2" max="2" width="120.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>662</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="9">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>599</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C8E61AB-16C5-45E5-BF34-9C7D74F0C910}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:I63"/>
   <sheetViews>

</xml_diff>